<commit_message>
Improved program. Runs autonomously well but not perfect
</commit_message>
<xml_diff>
--- a/Snake Game/Directions.xlsx
+++ b/Snake Game/Directions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loaya\Documents\Git Repositories\Home\Neural_Networks\Snake Game\Deep Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loaya\Documents\Git Repositories\Home\Neural_Networks\Snake Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE8480E-4273-4B48-926E-A4BC5953662C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97FC60B-B721-4EF2-B41E-56B02A7641AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8CDC4173-8F2A-4391-858E-0184FA750AAE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
   <si>
     <t>Left</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>#Front</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -486,7 +489,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -604,7 +610,10 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>